<commit_message>
Update JSClick class with safeclick method, refactored code and cleanup, completed Autocomplete search testing
</commit_message>
<xml_diff>
--- a/TestData/ColorSelection.xlsx
+++ b/TestData/ColorSelection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ASN\eclipse_workspace\demoqa-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE187DB7-A217-4028-A6A6-4A74EE98E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C05C5FD-9C42-49FC-9773-82DA05DD2B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,7 +669,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>